<commit_message>
Huge Update after last push
</commit_message>
<xml_diff>
--- a/company_data/Acre Data.xlsx
+++ b/company_data/Acre Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="main_variables"/>
@@ -13,7 +13,7 @@
     <sheet r:id="rId4" sheetId="4" name="dentist_contribution"/>
     <sheet r:id="rId5" sheetId="5" name="yearly_net_sales"/>
     <sheet r:id="rId6" sheetId="6" name="net_cash_flow"/>
-    <sheet r:id="rId7" sheetId="7" name="Copy of P&amp;amp;amp;amp;amp;amp;L_Ratio Rev 1.1_Model"/>
+    <sheet r:id="rId7" sheetId="7" name="Copy of P&amp;amp;amp;amp;amp;amp;amp;L_Ratio Rev 1.1_Model"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -1663,7 +1663,7 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1798,7 +1798,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="92">
-        <v>-319766</v>
+        <v>-308607</v>
       </c>
       <c r="E8" s="107"/>
       <c r="F8" s="108"/>
@@ -1926,7 +1926,7 @@
         <v>181</v>
       </c>
       <c r="D16" s="92">
-        <v>1045</v>
+        <v>1000</v>
       </c>
       <c r="E16" s="107"/>
       <c r="F16" s="108"/>
@@ -2191,7 +2191,7 @@
   </sheetPr>
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>